<commit_message>
added data for acm web and woot 2023
</commit_message>
<xml_diff>
--- a/call-for-artifacts-cleaned-data/WOOT-2019/WOOT-2019-ACCEPTED-REPO.xlsx
+++ b/call-for-artifacts-cleaned-data/WOOT-2019/WOOT-2019-ACCEPTED-REPO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workplace\artifact-evaluation-research\call-for-artifacts-cleaned-data\WOOT-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227FA27A-40BE-4851-94F7-0C9C4794D08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAED6BB-FCE2-4F8E-89A7-945DCF2DB1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27870" yWindow="4260" windowWidth="23040" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Research Paper Link</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Linked</t>
+  </si>
+  <si>
+    <t>Badge</t>
+  </si>
+  <si>
+    <t>Artifact Evaluated</t>
   </si>
 </sst>
 </file>
@@ -395,86 +401,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.5546875" customWidth="1"/>
+    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{200FA478-00A3-418A-BA11-3C1F9DC83F2E}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{013CE5A6-9171-49EB-8D51-17AE81705A78}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{013CE5A6-9171-49EB-8D51-17AE81705A78}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{847CCE44-E36F-416B-86EA-B0212AEB4402}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{429632A3-7D96-44DF-8D1F-A818B54DEA2C}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{429632A3-7D96-44DF-8D1F-A818B54DEA2C}"/>
     <hyperlink ref="A4" r:id="rId5" xr:uid="{26A309FF-7863-4D38-9F53-2626AD4829EC}"/>
-    <hyperlink ref="B4" r:id="rId6" xr:uid="{DE2CE851-A9F8-42A4-A985-DCF76F60FD99}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{DE2CE851-A9F8-42A4-A985-DCF76F60FD99}"/>
     <hyperlink ref="A5" r:id="rId7" xr:uid="{B53B27DF-8CE2-4FAA-8F18-600E935CCCB4}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{F6B6B80E-D0D3-4EF8-8362-AC05260A9A1C}"/>
-    <hyperlink ref="B6" r:id="rId9" xr:uid="{260C4634-A6E8-4DA1-9731-B67E169BFF17}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{F6B6B80E-D0D3-4EF8-8362-AC05260A9A1C}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{260C4634-A6E8-4DA1-9731-B67E169BFF17}"/>
     <hyperlink ref="A6" r:id="rId10" xr:uid="{B17E24D8-63BE-4F10-B3E3-B0DA4ED84D52}"/>
-    <hyperlink ref="C3" r:id="rId11" xr:uid="{7B69DAED-114B-4053-A2D2-B73929F62399}"/>
+    <hyperlink ref="D3" r:id="rId11" xr:uid="{7B69DAED-114B-4053-A2D2-B73929F62399}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>